<commit_message>
Project state table (#2420)
https://eao-dst.atlassian.net/browse/TRACK-177
1) Added Project State table
2) Endpoint to retrieve project states based on components
3) Updated the existing entries in the projects table for the column
project_state_id
4) Updated the action called set_project_state with the new change
5) Updated the action_configuration uses the old project state enum with
the new id
6) Updated Assessment and Exemptionrequest templates
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/assessment/002_EAC_Assessment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9AD25D-A25D-4207-95F2-85F617FB95E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFE9605-BB08-4726-8AB2-C51163E702DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1183,9 +1183,6 @@
     <t>{"phase_name":"EAC Decision","work_type_id": 6, "ea_act_id": 3, "event_name": "EAC Referral Package Received by Ministers", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"project_state": "PRE_CONSTRUCTION"}</t>
-  </si>
-  <si>
     <t>{"phase_name":"DPD Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of DPD Development", "start_at": 1 }</t>
   </si>
   <si>
@@ -1223,6 +1220,9 @@
   </si>
   <si>
     <t>{"phase_name":"Early Engagement","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"project_state_id": 13}</t>
   </si>
 </sst>
 </file>
@@ -2140,7 +2140,7 @@
         <v>303</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>9</v>
@@ -2169,7 +2169,7 @@
         <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
@@ -2198,7 +2198,7 @@
         <v>153</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>9</v>
@@ -2227,7 +2227,7 @@
         <v>154</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>9</v>
@@ -2256,7 +2256,7 @@
         <v>155</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>9</v>
@@ -2285,7 +2285,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>9</v>
@@ -2314,7 +2314,7 @@
         <v>157</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>9</v>
@@ -2343,7 +2343,7 @@
         <v>158</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>9</v>
@@ -2372,7 +2372,7 @@
         <v>159</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>9</v>
@@ -2401,7 +2401,7 @@
         <v>160</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>9</v>
@@ -2430,7 +2430,7 @@
         <v>161</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>9</v>
@@ -2459,7 +2459,7 @@
         <v>162</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>9</v>
@@ -16901,7 +16901,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -18160,10 +18160,10 @@
   <dimension ref="A1:G257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31:D145"/>
+      <selection pane="bottomRight" activeCell="F161" sqref="F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -18219,7 +18219,7 @@
         <v>296</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -18315,7 +18315,7 @@
         <v>302</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -18675,7 +18675,7 @@
         <v>296</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G21" s="2">
         <v>20</v>
@@ -18699,7 +18699,7 @@
         <v>296</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G22" s="2">
         <v>21</v>
@@ -18843,7 +18843,7 @@
         <v>314</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G28" s="2">
         <v>27</v>
@@ -18864,10 +18864,10 @@
         <v>85</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G29" s="2">
         <v>28</v>
@@ -18888,10 +18888,10 @@
         <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -19131,7 +19131,7 @@
         <v>316</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G40" s="2">
         <v>39</v>
@@ -19155,7 +19155,7 @@
         <v>296</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G41" s="2">
         <v>40</v>
@@ -19179,7 +19179,7 @@
         <v>296</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G42" s="2">
         <v>41</v>
@@ -19632,10 +19632,10 @@
         <v>97</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F61" s="70" t="s">
         <v>384</v>
-      </c>
-      <c r="F61" s="70" t="s">
-        <v>385</v>
       </c>
       <c r="G61" s="2">
         <v>60</v>
@@ -19851,7 +19851,7 @@
         <v>333</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G70" s="2">
         <v>69</v>
@@ -20376,10 +20376,10 @@
         <v>97</v>
       </c>
       <c r="E92" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="G92" s="2">
         <v>91</v>
@@ -20475,7 +20475,7 @@
         <v>333</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G96" s="2">
         <v>95</v>
@@ -20547,7 +20547,7 @@
         <v>333</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G99" s="2">
         <v>98</v>
@@ -20811,7 +20811,7 @@
         <v>296</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G110" s="2">
         <v>109</v>
@@ -20835,7 +20835,7 @@
         <v>296</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G111" s="2">
         <v>110</v>
@@ -21315,7 +21315,7 @@
         <v>296</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G131" s="2">
         <v>130</v>
@@ -21339,7 +21339,7 @@
         <v>296</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G132" s="2">
         <v>131</v>
@@ -21600,10 +21600,10 @@
         <v>85</v>
       </c>
       <c r="E143" s="68" t="s">
+        <v>385</v>
+      </c>
+      <c r="F143" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="G143" s="2">
         <v>142</v>
@@ -22011,7 +22011,7 @@
         <v>341</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>379</v>
+        <v>392</v>
       </c>
       <c r="G160" s="2">
         <v>159</v>
@@ -23333,7 +23333,7 @@
     </row>
     <row r="6" spans="1:59">
       <c r="B6" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>24</v>
@@ -24783,14 +24783,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25023,21 +25021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25062,9 +25059,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37DBE489-EE2E-427D-B9CD-0FAE2F0995FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB0BEEB2-93D8-45BE-86D5-11172DAC5CD0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>